<commit_message>
first two instructions working
</commit_message>
<xml_diff>
--- a/control LUT generator.xlsx
+++ b/control LUT generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Chris\Downloads\8 bit computer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9245F14-1D9C-42D5-BC97-FB4458A28782}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{164BAB86-67BF-4CA0-8626-3FD890803317}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{DAB1FA04-CE66-4B0E-BC0E-6E0D84A24BB7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>bit number</t>
   </si>
@@ -147,31 +147,10 @@
     <t>function (control pin)</t>
   </si>
   <si>
-    <t>Enable write 1</t>
-  </si>
-  <si>
-    <t>Enable write 2</t>
-  </si>
-  <si>
-    <t>Enable write 3</t>
-  </si>
-  <si>
-    <t>Enable write 4</t>
-  </si>
-  <si>
     <t>Clear registers</t>
   </si>
   <si>
-    <t>!Load PC MSB</t>
-  </si>
-  <si>
-    <t>!Load PC LSB</t>
-  </si>
-  <si>
     <t>Load Saved PC</t>
-  </si>
-  <si>
-    <t>!Equal Zero</t>
   </si>
   <si>
     <t>Subtract / !Add</t>
@@ -195,19 +174,43 @@
     <t>OCL Enable Reg</t>
   </si>
   <si>
-    <t>! Enable Interrupts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass Write Mux </t>
-  </si>
-  <si>
-    <t>Pass Read Mux 1</t>
-  </si>
-  <si>
     <t>Pass Read Mux 2</t>
   </si>
   <si>
-    <t>!Load PC LSB &amp; Equal Zero ( for JNZ...)</t>
+    <t>RAM Write To</t>
+  </si>
+  <si>
+    <t>Enable Register Write</t>
+  </si>
+  <si>
+    <t>Pass Read Mux 1 (pass from instruciton)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Mux Bit 4 </t>
+  </si>
+  <si>
+    <t>Write Mux Bit 3</t>
+  </si>
+  <si>
+    <t>Write Mux Bit 2</t>
+  </si>
+  <si>
+    <t>Write Mux Bit 1</t>
+  </si>
+  <si>
+    <t>Load PC MSB</t>
+  </si>
+  <si>
+    <t>Equal Zero</t>
+  </si>
+  <si>
+    <t>Load PC LSB &amp; Equal Zero ( for JNZ...)</t>
+  </si>
+  <si>
+    <t>Load PC LSB</t>
+  </si>
+  <si>
+    <t>Disable Interrupts</t>
   </si>
 </sst>
 </file>
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C70AF1-ED50-4B9F-9B65-C4215ACAA671}">
   <dimension ref="A2:AM140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM16" sqref="AM16"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM30" sqref="AM30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,7 @@
     <col min="36" max="36" width="15.7109375" customWidth="1"/>
     <col min="37" max="37" width="16.5703125" customWidth="1"/>
     <col min="38" max="38" width="14.85546875" customWidth="1"/>
-    <col min="39" max="39" width="37.85546875" customWidth="1"/>
+    <col min="39" max="39" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -821,14 +824,14 @@
       <c r="K5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="3">
         <v>0</v>
       </c>
       <c r="M5" s="3">
         <v>0</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="3">
         <v>0</v>
@@ -870,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="3">
         <v>0</v>
@@ -882,18 +885,18 @@
         <v>0</v>
       </c>
       <c r="AF5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" s="3">
         <v>0</v>
       </c>
       <c r="AI5">
         <f>SUM(B75:AG75)</f>
-        <v>0</v>
+        <v>1140854784</v>
       </c>
       <c r="AJ5" t="str">
         <f>DEC2HEX(AI5)</f>
-        <v>0</v>
+        <v>44001000</v>
       </c>
       <c r="AL5">
         <v>1</v>
@@ -936,79 +939,79 @@
       <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="3">
         <v>0</v>
       </c>
       <c r="M6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3">
         <v>1</v>
       </c>
       <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
         <v>1</v>
       </c>
-      <c r="P6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>11</v>
-      </c>
-      <c r="R6" s="3">
-        <v>1</v>
-      </c>
-      <c r="S6" s="3">
-        <v>1</v>
-      </c>
-      <c r="T6" s="3">
-        <v>1</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>0</v>
-      </c>
       <c r="AC6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="3">
         <v>0</v>
       </c>
       <c r="AE6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="3">
         <v>1</v>
       </c>
       <c r="AG6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6">
         <f t="shared" ref="AI6:AI69" si="0">SUM(B76:AG76)</f>
-        <v>3893164032</v>
+        <v>1140854784</v>
       </c>
       <c r="AJ6" t="str">
         <f t="shared" ref="AJ6:AJ69" si="1">DEC2HEX(AI6)</f>
-        <v>E80CF800</v>
+        <v>44001000</v>
       </c>
       <c r="AL6">
         <v>2</v>
@@ -1051,7 +1054,7 @@
       <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="3">
         <v>0</v>
       </c>
       <c r="M7" s="3"/>
@@ -1124,7 +1127,7 @@
       <c r="K8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="3">
         <v>0</v>
       </c>
       <c r="M8" s="3"/>
@@ -1197,7 +1200,7 @@
       <c r="K9" s="2">
         <v>0</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="3">
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
@@ -1270,7 +1273,7 @@
       <c r="K10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="3">
         <v>0</v>
       </c>
       <c r="M10" s="3"/>
@@ -1343,7 +1346,7 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="3">
         <v>0</v>
       </c>
       <c r="M11" s="3"/>
@@ -1416,7 +1419,7 @@
       <c r="K12" s="2">
         <v>0</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="3">
         <v>0</v>
       </c>
       <c r="M12" s="3"/>
@@ -1489,7 +1492,7 @@
       <c r="K13" s="2">
         <v>0</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="3">
         <v>0</v>
       </c>
       <c r="M13" s="3"/>
@@ -1562,7 +1565,7 @@
       <c r="K14" s="2">
         <v>0</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="3">
         <v>0</v>
       </c>
       <c r="M14" s="3"/>
@@ -1598,7 +1601,7 @@
         <v>10</v>
       </c>
       <c r="AM14" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1635,7 +1638,7 @@
       <c r="K15" s="2">
         <v>0</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="3">
         <v>0</v>
       </c>
       <c r="M15" s="3"/>
@@ -1671,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="AM15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1708,7 +1711,7 @@
       <c r="K16" s="2">
         <v>0</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="3">
         <v>0</v>
       </c>
       <c r="M16" s="3"/>
@@ -1744,7 +1747,7 @@
         <v>12</v>
       </c>
       <c r="AM16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1781,7 +1784,7 @@
       <c r="K17" s="2">
         <v>0</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="3">
         <v>0</v>
       </c>
       <c r="M17" s="3"/>
@@ -1817,7 +1820,7 @@
         <v>13</v>
       </c>
       <c r="AM17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1854,7 +1857,7 @@
       <c r="K18" s="2">
         <v>0</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="3">
         <v>0</v>
       </c>
       <c r="M18" s="3"/>
@@ -1890,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="AM18" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1927,7 +1930,7 @@
       <c r="K19" s="2">
         <v>0</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="3">
         <v>0</v>
       </c>
       <c r="M19" s="3"/>
@@ -1963,7 +1966,7 @@
         <v>15</v>
       </c>
       <c r="AM19" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2000,7 +2003,7 @@
       <c r="K20" s="2">
         <v>0</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="3">
         <v>0</v>
       </c>
       <c r="M20" s="3"/>
@@ -2036,7 +2039,7 @@
         <v>16</v>
       </c>
       <c r="AM20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2073,7 +2076,7 @@
       <c r="K21" s="2">
         <v>0</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="3">
         <v>0</v>
       </c>
       <c r="M21" s="3"/>
@@ -2109,7 +2112,7 @@
         <v>17</v>
       </c>
       <c r="AM21" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2146,7 +2149,7 @@
       <c r="K22" s="2">
         <v>0</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="3">
         <v>0</v>
       </c>
       <c r="M22" s="3"/>
@@ -2182,7 +2185,7 @@
         <v>18</v>
       </c>
       <c r="AM22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2219,7 +2222,7 @@
       <c r="K23" s="2">
         <v>0</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="3">
         <v>0</v>
       </c>
       <c r="M23" s="3"/>
@@ -2255,7 +2258,7 @@
         <v>19</v>
       </c>
       <c r="AM23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2292,7 +2295,7 @@
       <c r="K24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="3">
         <v>0</v>
       </c>
       <c r="M24" s="3"/>
@@ -2328,7 +2331,7 @@
         <v>20</v>
       </c>
       <c r="AM24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2365,7 +2368,7 @@
       <c r="K25" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="3">
         <v>0</v>
       </c>
       <c r="M25" s="3"/>
@@ -2401,7 +2404,7 @@
         <v>21</v>
       </c>
       <c r="AM25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2438,7 +2441,7 @@
       <c r="K26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="3">
         <v>0</v>
       </c>
       <c r="M26" s="3"/>
@@ -2474,7 +2477,7 @@
         <v>22</v>
       </c>
       <c r="AM26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2514,7 @@
       <c r="K27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="3">
         <v>0</v>
       </c>
       <c r="M27" s="3"/>
@@ -2547,7 +2550,7 @@
         <v>23</v>
       </c>
       <c r="AM27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2584,7 +2587,7 @@
       <c r="K28" s="2">
         <v>0</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="3">
         <v>0</v>
       </c>
       <c r="M28" s="3"/>
@@ -2620,7 +2623,7 @@
         <v>24</v>
       </c>
       <c r="AM28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2657,7 +2660,7 @@
       <c r="K29" s="2">
         <v>0</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="3">
         <v>0</v>
       </c>
       <c r="M29" s="3"/>
@@ -2693,7 +2696,7 @@
         <v>25</v>
       </c>
       <c r="AM29" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2730,7 +2733,7 @@
       <c r="K30" s="2">
         <v>0</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="3">
         <v>0</v>
       </c>
       <c r="M30" s="3"/>
@@ -2766,7 +2769,7 @@
         <v>26</v>
       </c>
       <c r="AM30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2803,7 +2806,7 @@
       <c r="K31" s="2">
         <v>0</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="3">
         <v>0</v>
       </c>
       <c r="M31" s="3"/>
@@ -2876,7 +2879,7 @@
       <c r="K32" s="2">
         <v>0</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="3">
         <v>0</v>
       </c>
       <c r="M32" s="3"/>
@@ -2912,7 +2915,7 @@
         <v>28</v>
       </c>
       <c r="AM32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2949,7 +2952,7 @@
       <c r="K33" s="2">
         <v>0</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="3">
         <v>0</v>
       </c>
       <c r="M33" s="3"/>
@@ -2985,7 +2988,7 @@
         <v>29</v>
       </c>
       <c r="AM33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3022,7 +3025,7 @@
       <c r="K34" s="2">
         <v>0</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="3">
         <v>0</v>
       </c>
       <c r="M34" s="3"/>
@@ -3058,7 +3061,7 @@
         <v>30</v>
       </c>
       <c r="AM34" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3095,7 +3098,7 @@
       <c r="K35" s="2">
         <v>0</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="3">
         <v>0</v>
       </c>
       <c r="M35" s="3"/>
@@ -3131,7 +3134,7 @@
         <v>31</v>
       </c>
       <c r="AM35" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3168,7 +3171,7 @@
       <c r="K36" s="2">
         <v>0</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="3">
         <v>0</v>
       </c>
       <c r="M36" s="3"/>
@@ -3232,7 +3235,7 @@
       <c r="K37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="3">
         <v>0</v>
       </c>
       <c r="M37" s="3"/>
@@ -3296,7 +3299,7 @@
       <c r="K38" s="2">
         <v>0</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="3">
         <v>0</v>
       </c>
       <c r="M38" s="3"/>
@@ -3360,7 +3363,7 @@
       <c r="K39" s="2">
         <v>0</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="3">
         <v>0</v>
       </c>
       <c r="M39" s="3"/>
@@ -3424,7 +3427,7 @@
       <c r="K40" s="2">
         <v>0</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="3">
         <v>0</v>
       </c>
       <c r="M40" s="3"/>
@@ -3488,7 +3491,7 @@
       <c r="K41" s="2">
         <v>0</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="3">
         <v>0</v>
       </c>
       <c r="M41" s="3"/>
@@ -3552,7 +3555,7 @@
       <c r="K42" s="2">
         <v>0</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="3">
         <v>0</v>
       </c>
       <c r="M42" s="3"/>
@@ -3616,7 +3619,7 @@
       <c r="K43" s="2">
         <v>0</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L43" s="3">
         <v>0</v>
       </c>
       <c r="M43" s="3"/>
@@ -3680,7 +3683,7 @@
       <c r="K44" s="2">
         <v>0</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="3">
         <v>0</v>
       </c>
       <c r="M44" s="3"/>
@@ -3744,7 +3747,7 @@
       <c r="K45" s="2">
         <v>0</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="3">
         <v>0</v>
       </c>
       <c r="M45" s="3"/>
@@ -3808,7 +3811,7 @@
       <c r="K46" s="2">
         <v>0</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="3">
         <v>0</v>
       </c>
       <c r="M46" s="3"/>
@@ -3872,7 +3875,7 @@
       <c r="K47" s="2">
         <v>0</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L47" s="3">
         <v>0</v>
       </c>
       <c r="M47" s="3"/>
@@ -3936,7 +3939,7 @@
       <c r="K48" s="2">
         <v>0</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="3">
         <v>0</v>
       </c>
       <c r="M48" s="3"/>
@@ -4000,7 +4003,7 @@
       <c r="K49" s="2">
         <v>0</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L49" s="3">
         <v>0</v>
       </c>
       <c r="M49" s="3"/>
@@ -4064,7 +4067,7 @@
       <c r="K50" s="2">
         <v>0</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L50" s="3">
         <v>0</v>
       </c>
       <c r="M50" s="3"/>
@@ -4128,7 +4131,7 @@
       <c r="K51" s="2">
         <v>0</v>
       </c>
-      <c r="L51" s="2">
+      <c r="L51" s="3">
         <v>0</v>
       </c>
       <c r="M51" s="3"/>
@@ -4192,7 +4195,7 @@
       <c r="K52" s="2">
         <v>0</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L52" s="3">
         <v>0</v>
       </c>
       <c r="M52" s="3"/>
@@ -4256,7 +4259,7 @@
       <c r="K53" s="2">
         <v>0</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L53" s="3">
         <v>0</v>
       </c>
       <c r="M53" s="3"/>
@@ -4320,7 +4323,7 @@
       <c r="K54" s="2">
         <v>0</v>
       </c>
-      <c r="L54" s="2">
+      <c r="L54" s="3">
         <v>0</v>
       </c>
       <c r="M54" s="3"/>
@@ -4384,7 +4387,7 @@
       <c r="K55" s="2">
         <v>0</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="3">
         <v>0</v>
       </c>
       <c r="M55" s="3"/>
@@ -4448,7 +4451,7 @@
       <c r="K56" s="2">
         <v>0</v>
       </c>
-      <c r="L56" s="2">
+      <c r="L56" s="3">
         <v>0</v>
       </c>
       <c r="M56" s="3"/>
@@ -4512,7 +4515,7 @@
       <c r="K57" s="2">
         <v>0</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="3">
         <v>0</v>
       </c>
       <c r="M57" s="3"/>
@@ -4576,7 +4579,7 @@
       <c r="K58" s="2">
         <v>0</v>
       </c>
-      <c r="L58" s="2">
+      <c r="L58" s="3">
         <v>0</v>
       </c>
       <c r="M58" s="3"/>
@@ -4640,7 +4643,7 @@
       <c r="K59" s="2">
         <v>0</v>
       </c>
-      <c r="L59" s="2">
+      <c r="L59" s="3">
         <v>0</v>
       </c>
       <c r="M59" s="3"/>
@@ -4704,7 +4707,7 @@
       <c r="K60" s="2">
         <v>0</v>
       </c>
-      <c r="L60" s="2">
+      <c r="L60" s="3">
         <v>0</v>
       </c>
       <c r="M60" s="3"/>
@@ -4768,7 +4771,7 @@
       <c r="K61" s="2">
         <v>0</v>
       </c>
-      <c r="L61" s="2">
+      <c r="L61" s="3">
         <v>0</v>
       </c>
       <c r="M61" s="3"/>
@@ -4832,7 +4835,7 @@
       <c r="K62" s="2">
         <v>0</v>
       </c>
-      <c r="L62" s="2">
+      <c r="L62" s="3">
         <v>0</v>
       </c>
       <c r="M62" s="3"/>
@@ -4896,7 +4899,7 @@
       <c r="K63" s="2">
         <v>0</v>
       </c>
-      <c r="L63" s="2">
+      <c r="L63" s="3">
         <v>0</v>
       </c>
       <c r="M63" s="3"/>
@@ -4960,7 +4963,7 @@
       <c r="K64" s="2">
         <v>0</v>
       </c>
-      <c r="L64" s="2">
+      <c r="L64" s="3">
         <v>0</v>
       </c>
       <c r="M64" s="3"/>
@@ -5024,7 +5027,7 @@
       <c r="K65" s="2">
         <v>0</v>
       </c>
-      <c r="L65" s="2">
+      <c r="L65" s="3">
         <v>0</v>
       </c>
       <c r="M65" s="3"/>
@@ -5088,7 +5091,7 @@
       <c r="K66" s="2">
         <v>0</v>
       </c>
-      <c r="L66" s="2">
+      <c r="L66" s="3">
         <v>0</v>
       </c>
       <c r="M66" s="3"/>
@@ -5152,7 +5155,7 @@
       <c r="K67" s="2">
         <v>0</v>
       </c>
-      <c r="L67" s="2">
+      <c r="L67" s="3">
         <v>0</v>
       </c>
       <c r="M67" s="3"/>
@@ -5216,7 +5219,7 @@
       <c r="K68" s="2">
         <v>0</v>
       </c>
-      <c r="L68" s="2">
+      <c r="L68" s="3">
         <v>0</v>
       </c>
       <c r="M68" s="3"/>
@@ -5280,7 +5283,7 @@
       <c r="K69" s="2">
         <v>0</v>
       </c>
-      <c r="L69" s="2">
+      <c r="L69" s="3">
         <v>0</v>
       </c>
       <c r="M69" s="3"/>
@@ -5344,7 +5347,7 @@
       <c r="K70" s="2">
         <v>0</v>
       </c>
-      <c r="L70" s="2">
+      <c r="L70" s="3">
         <v>0</v>
       </c>
       <c r="M70" s="3"/>
@@ -5433,7 +5436,7 @@
       </c>
       <c r="N75">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="O75">
         <f t="shared" si="4"/>
@@ -5489,7 +5492,7 @@
       </c>
       <c r="AB75">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>67108864</v>
       </c>
       <c r="AC75">
         <f t="shared" si="4"/>
@@ -5505,7 +5508,7 @@
       </c>
       <c r="AF75">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1073741824</v>
       </c>
       <c r="AG75">
         <f t="shared" si="4"/>
@@ -5559,7 +5562,7 @@
       </c>
       <c r="M76">
         <f t="shared" si="6"/>
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="N76">
         <f t="shared" si="6"/>
@@ -5567,27 +5570,27 @@
       </c>
       <c r="O76">
         <f t="shared" si="6"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="P76">
         <f t="shared" si="6"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
       <c r="Q76">
         <f t="shared" si="6"/>
-        <v>360448</v>
+        <v>0</v>
       </c>
       <c r="R76">
         <f t="shared" si="6"/>
-        <v>65536</v>
+        <v>0</v>
       </c>
       <c r="S76">
         <f t="shared" si="6"/>
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="T76">
         <f t="shared" si="6"/>
-        <v>262144</v>
+        <v>0</v>
       </c>
       <c r="U76">
         <f t="shared" si="6"/>
@@ -5619,11 +5622,11 @@
       </c>
       <c r="AB76">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>67108864</v>
       </c>
       <c r="AC76">
         <f t="shared" si="6"/>
-        <v>134217728</v>
+        <v>0</v>
       </c>
       <c r="AD76">
         <f t="shared" si="6"/>
@@ -5631,7 +5634,7 @@
       </c>
       <c r="AE76">
         <f t="shared" si="6"/>
-        <v>536870912</v>
+        <v>0</v>
       </c>
       <c r="AF76">
         <f t="shared" si="6"/>
@@ -5639,7 +5642,7 @@
       </c>
       <c r="AG76">
         <f t="shared" si="6"/>
-        <v>2147483648</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>